<commit_message>
Got rid of extra whitespace in the expected result column which causes tests to fail.
</commit_message>
<xml_diff>
--- a/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
+++ b/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="-10300" yWindow="-19680" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>test_case_id</t>
   </si>
@@ -37,12 +37,6 @@
     <t xml:space="preserve">expected_result </t>
   </si>
   <si>
-    <t xml:space="preserve">success </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fail </t>
-  </si>
-  <si>
     <t xml:space="preserve">invalid_mapping_invalid_id </t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>54321</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -114,8 +114,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -158,7 +168,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -177,6 +187,11 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -195,6 +210,11 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,21 +544,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,53 +565,47 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -613,13 +621,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Tested and updated test data files
</commit_message>
<xml_diff>
--- a/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
+++ b/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-10300" yWindow="-19680" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="legends" sheetId="2" r:id="rId2"/>
+    <sheet name="Test data notes" sheetId="3" r:id="rId3"/>
+    <sheet name="backup" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>test_case_id</t>
   </si>
@@ -37,35 +39,122 @@
     <t xml:space="preserve">expected_result </t>
   </si>
   <si>
-    <t xml:space="preserve">invalid_mapping_invalid_id </t>
-  </si>
-  <si>
-    <t xml:space="preserve">invalid_mapping_previously_mapped </t>
-  </si>
-  <si>
-    <t>331310</t>
-  </si>
-  <si>
-    <t>334593</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>54321</t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>expected_alert_text</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>not be crosslisted</t>
+  </si>
+  <si>
+    <t>327828</t>
+  </si>
+  <si>
+    <t>336841</t>
+  </si>
+  <si>
+    <t>successfully crosslisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fail_mapping_invalid_id </t>
+  </si>
+  <si>
+    <t>already crosslisted</t>
+  </si>
+  <si>
+    <t>fail_mapping_already_exists</t>
+  </si>
+  <si>
+    <t>fail_if_secondary_is_primary_for_another</t>
+  </si>
+  <si>
+    <t>currently crosslisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fail_reverse_mapping </t>
+  </si>
+  <si>
+    <t>reverse pairing</t>
+  </si>
+  <si>
+    <t>Covered by test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messages </t>
+  </si>
+  <si>
+    <t>"A reverse pairing for these IDs (primary:334009, secondary:336003) already exists"</t>
+  </si>
+  <si>
+    <t>"12345 is already crosslisted with 34567"</t>
+  </si>
+  <si>
+    <t>If pair already exists</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>If the secondary course is a primary for another course</t>
+  </si>
+  <si>
+    <t>"34567 is currently crosslisted with 89072 as a primary"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All others </t>
+  </si>
+  <si>
+    <t>"12345 could not be crosslisted with 34567 at this time. Please check the course instance IDs and try again"</t>
+  </si>
+  <si>
+    <t>If reverse mapping already exists</t>
+  </si>
+  <si>
+    <t>333313</t>
+  </si>
+  <si>
+    <t>330548</t>
+  </si>
+  <si>
+    <t>339433</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For most of the tests, as long as these ID are cross listed, the tests should work </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the expected failed tests </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the success (any two CID with Canvas course should do) </t>
+  </si>
+  <si>
+    <t>355757</t>
+  </si>
+  <si>
+    <t>355756</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +185,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FF808080"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +235,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,13 +283,121 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -192,6 +421,56 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -215,6 +494,56 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,69 +873,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="63.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="H11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -621,68 +1006,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -694,4 +1083,191 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="111.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addressed all the issues with remove tests per PR feedback. Tested locally.
</commit_message>
<xml_diff>
--- a/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
+++ b/selenium_tests/cross_listing/test_data/cross_listing_mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-16960" yWindow="-17520" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -144,10 +144,10 @@
     <t xml:space="preserve">For the success (any two CID with Canvas course should do) </t>
   </si>
   <si>
-    <t>355757</t>
-  </si>
-  <si>
-    <t>355756</t>
+    <t>342124</t>
+  </si>
+  <si>
+    <t>341756</t>
   </si>
 </sst>
 </file>
@@ -235,8 +235,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -397,7 +401,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -471,6 +475,8 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -544,6 +550,8 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -875,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:E6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1150,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1264,6 +1272,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>